<commit_message>
Update: Cambios en generacion de reporte de vales
</commit_message>
<xml_diff>
--- a/public/archivos/formatoReporteSolicitudValesV5.xlsx
+++ b/public/archivos/formatoReporteSolicitudValesV5.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diegolopez/Documents/GitProyect/vales/apivales/public/archivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CD090C-A7E6-2B4E-A3AF-48D72CDB51DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C8AE10-4D66-3041-9296-320F3D336965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="27820" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Solicitudes Vales Grandeza" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Solicitudes Vales Grandeza'!$A$2:$AK$48</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Solicitudes Vales Grandeza'!$A$2:$AC$48</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Solicitudes Vales Grandeza'!$2:$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>NO.</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Sexo</t>
   </si>
   <si>
-    <t>FechaNacimiento</t>
-  </si>
-  <si>
     <t>TelFijo</t>
   </si>
   <si>
@@ -84,24 +81,6 @@
     <t>Capturo</t>
   </si>
   <si>
-    <t>Tel Recados</t>
-  </si>
-  <si>
-    <t>Ocuapción</t>
-  </si>
-  <si>
-    <t>Ingreso Percibido</t>
-  </si>
-  <si>
-    <t>Otros Ingresos</t>
-  </si>
-  <si>
-    <t>Total Ingresos</t>
-  </si>
-  <si>
-    <t>Personas</t>
-  </si>
-  <si>
     <t>Incidencia</t>
   </si>
   <si>
@@ -135,16 +114,13 @@
     <t>Actualizo</t>
   </si>
   <si>
-    <t>FolioImpulso</t>
-  </si>
-  <si>
-    <t>FolioVales</t>
-  </si>
-  <si>
     <t>Paterno</t>
   </si>
   <si>
     <t>Materno</t>
+  </si>
+  <si>
+    <t>FolioSolicitud</t>
   </si>
 </sst>
 </file>
@@ -237,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -248,12 +224,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -269,9 +239,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -279,15 +246,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -320,8 +278,8 @@
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>69374</xdr:rowOff>
     </xdr:to>
@@ -633,10 +591,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK10"/>
+  <dimension ref="A1:AC10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -645,74 +603,59 @@
     <col min="2" max="2" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
     <col min="4" max="4" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="26" customWidth="1"/>
-    <col min="9" max="9" width="25.83203125" customWidth="1"/>
-    <col min="10" max="10" width="20.5" customWidth="1"/>
-    <col min="11" max="11" width="21.5" customWidth="1"/>
-    <col min="12" max="12" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5" customWidth="1"/>
-    <col min="14" max="14" width="38.6640625" customWidth="1"/>
-    <col min="15" max="15" width="20.5" customWidth="1"/>
-    <col min="16" max="16" width="20.83203125" customWidth="1"/>
-    <col min="17" max="18" width="6.83203125" customWidth="1"/>
-    <col min="19" max="19" width="9.83203125" customWidth="1"/>
-    <col min="20" max="20" width="25.83203125" customWidth="1"/>
-    <col min="21" max="23" width="30.83203125" customWidth="1"/>
-    <col min="24" max="26" width="12.83203125" customWidth="1"/>
-    <col min="27" max="27" width="33.33203125" customWidth="1"/>
-    <col min="28" max="28" width="17.33203125" customWidth="1"/>
-    <col min="29" max="29" width="18.1640625" customWidth="1"/>
-    <col min="30" max="30" width="18.33203125" customWidth="1"/>
-    <col min="31" max="31" width="14.5" customWidth="1"/>
-    <col min="32" max="32" width="29.5" customWidth="1"/>
-    <col min="33" max="34" width="14.5" customWidth="1"/>
-    <col min="35" max="36" width="15.83203125" customWidth="1"/>
-    <col min="37" max="37" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="26" customWidth="1"/>
+    <col min="8" max="8" width="25.83203125" customWidth="1"/>
+    <col min="9" max="9" width="20.5" customWidth="1"/>
+    <col min="10" max="10" width="21.5" customWidth="1"/>
+    <col min="11" max="11" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.5" customWidth="1"/>
+    <col min="13" max="13" width="20.83203125" customWidth="1"/>
+    <col min="14" max="15" width="6.83203125" customWidth="1"/>
+    <col min="16" max="16" width="9.83203125" customWidth="1"/>
+    <col min="17" max="17" width="25.83203125" customWidth="1"/>
+    <col min="18" max="20" width="30.83203125" customWidth="1"/>
+    <col min="21" max="22" width="12.83203125" customWidth="1"/>
+    <col min="23" max="23" width="33.33203125" customWidth="1"/>
+    <col min="24" max="24" width="29.5" customWidth="1"/>
+    <col min="25" max="26" width="14.5" customWidth="1"/>
+    <col min="27" max="28" width="15.83203125" customWidth="1"/>
+    <col min="29" max="29" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="11"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
       <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
       <c r="AA1" s="3"/>
-      <c r="AB1" s="11"/>
-      <c r="AC1" s="11"/>
-      <c r="AD1" s="11"/>
-      <c r="AE1" s="11"/>
-      <c r="AF1" s="15"/>
-      <c r="AG1" s="15"/>
-      <c r="AH1" s="15"/>
-      <c r="AI1" s="15"/>
-      <c r="AJ1" s="16"/>
-      <c r="AK1" s="15"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -725,33 +668,25 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="11"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
       <c r="S2" s="6"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6"/>
-      <c r="AE2" s="6"/>
-      <c r="AF2" s="6"/>
-      <c r="AG2" s="6"/>
-      <c r="AH2" s="6"/>
-      <c r="AI2" s="6"/>
-      <c r="AJ2" s="6"/>
-      <c r="AK2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -763,34 +698,26 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
-      <c r="W3" s="9"/>
-      <c r="X3" s="9"/>
-      <c r="Y3" s="9"/>
-      <c r="Z3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
       <c r="AA3" s="3"/>
-      <c r="AB3" s="11"/>
-      <c r="AC3" s="11"/>
-      <c r="AD3" s="11"/>
-      <c r="AE3" s="11"/>
-      <c r="AF3" s="15"/>
-      <c r="AG3" s="15"/>
-      <c r="AH3" s="15"/>
-      <c r="AI3" s="15"/>
-      <c r="AJ3" s="16"/>
-      <c r="AK3" s="15"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -802,34 +729,26 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9"/>
-      <c r="X4" s="9"/>
-      <c r="Y4" s="9"/>
-      <c r="Z4" s="9"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
-      <c r="AB4" s="11"/>
-      <c r="AC4" s="11"/>
-      <c r="AD4" s="11"/>
-      <c r="AE4" s="11"/>
-      <c r="AF4" s="15"/>
-      <c r="AG4" s="15"/>
-      <c r="AH4" s="15"/>
-      <c r="AI4" s="15"/>
-      <c r="AJ4" s="16"/>
-      <c r="AK4" s="15"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -841,34 +760,26 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="3"/>
       <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="9"/>
-      <c r="W5" s="9"/>
-      <c r="X5" s="9"/>
-      <c r="Y5" s="9"/>
-      <c r="Z5" s="9"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
-      <c r="AB5" s="11"/>
-      <c r="AC5" s="11"/>
-      <c r="AD5" s="11"/>
-      <c r="AE5" s="11"/>
-      <c r="AF5" s="15"/>
-      <c r="AG5" s="15"/>
-      <c r="AH5" s="15"/>
-      <c r="AI5" s="15"/>
-      <c r="AJ5" s="16"/>
-      <c r="AK5" s="15"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -881,33 +792,25 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="11"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
       <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="9"/>
-      <c r="Y6" s="9"/>
-      <c r="Z6" s="9"/>
-      <c r="AA6" s="18"/>
-      <c r="AB6" s="18"/>
-      <c r="AC6" s="18"/>
-      <c r="AD6" s="18"/>
-      <c r="AE6" s="18"/>
-      <c r="AF6" s="18"/>
-      <c r="AG6" s="18"/>
-      <c r="AH6" s="18"/>
-      <c r="AI6" s="18"/>
-      <c r="AJ6" s="18"/>
-      <c r="AK6" s="18"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="12"/>
+      <c r="AA6" s="12"/>
+      <c r="AB6" s="12"/>
+      <c r="AC6" s="12"/>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -920,33 +823,25 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="11"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
       <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="9"/>
-      <c r="W7" s="9"/>
-      <c r="X7" s="9"/>
-      <c r="Y7" s="9"/>
-      <c r="Z7" s="9"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
       <c r="AA7" s="3"/>
-      <c r="AB7" s="11"/>
-      <c r="AC7" s="11"/>
-      <c r="AD7" s="11"/>
-      <c r="AE7" s="11"/>
-      <c r="AF7" s="15"/>
-      <c r="AG7" s="15"/>
-      <c r="AH7" s="15"/>
-      <c r="AI7" s="15"/>
-      <c r="AJ7" s="16"/>
-      <c r="AK7" s="15"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -958,186 +853,146 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
+      <c r="L8" s="3"/>
       <c r="M8" s="3"/>
-      <c r="N8" s="11"/>
+      <c r="N8" s="3"/>
       <c r="O8" s="3"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="9"/>
-      <c r="U8" s="9"/>
-      <c r="V8" s="9"/>
-      <c r="W8" s="9"/>
-      <c r="X8" s="9"/>
-      <c r="Y8" s="9"/>
-      <c r="Z8" s="9"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
       <c r="AA8" s="3"/>
-      <c r="AB8" s="11"/>
-      <c r="AC8" s="11"/>
-      <c r="AD8" s="11"/>
-      <c r="AE8" s="11"/>
-      <c r="AF8" s="15"/>
-      <c r="AG8" s="15"/>
-      <c r="AH8" s="15"/>
-      <c r="AI8" s="15"/>
-      <c r="AJ8" s="16"/>
-      <c r="AK8" s="15"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="17"/>
+      <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
-      <c r="N9" s="11"/>
+      <c r="N9" s="3"/>
       <c r="O9" s="3"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="9"/>
-      <c r="V9" s="9"/>
-      <c r="W9" s="9"/>
-      <c r="X9" s="9"/>
-      <c r="Y9" s="9"/>
-      <c r="Z9" s="9"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
       <c r="AA9" s="3"/>
-      <c r="AB9" s="11"/>
-      <c r="AC9" s="11"/>
-      <c r="AD9" s="11"/>
-      <c r="AE9" s="11"/>
-      <c r="AF9" s="15"/>
-      <c r="AG9" s="15"/>
-      <c r="AH9" s="15"/>
-      <c r="AI9" s="15"/>
-      <c r="AJ9" s="16"/>
-      <c r="AK9" s="15"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
     </row>
-    <row r="10" spans="1:37" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
-      <c r="B10" s="14" t="s">
+    <row r="10" spans="1:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+      <c r="B10" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="14" t="s">
+      <c r="C10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="14" t="s">
+      <c r="E10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="G10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="H10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="K10" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="L10" s="14" t="s">
+      <c r="I10" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M10" s="14" t="s">
+      <c r="L10" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="O10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="P10" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="R10" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="S10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="T10" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="U10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="N10" s="14" t="s">
+      <c r="V10" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="W10" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="X10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC10" s="11" t="s">
         <v>16</v>
-      </c>
-      <c r="O10" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="P10" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q10" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="R10" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="S10" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="T10" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="U10" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="V10" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="W10" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="X10" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y10" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z10" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA10" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB10" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="AC10" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="AD10" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE10" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="AF10" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="AG10" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH10" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI10" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="AJ10" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="AK10" s="14" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="AA6:AK6"/>
+    <mergeCell ref="W6:AC6"/>
   </mergeCells>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
   <pageSetup scale="30" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Add: Se agregó módulo de reimpresión de acuse individual
</commit_message>
<xml_diff>
--- a/public/archivos/formatoReporteSolicitudValesV5.xlsx
+++ b/public/archivos/formatoReporteSolicitudValesV5.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diegolopez/Documents/GitProyect/vales/apivales/public/archivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C8AE10-4D66-3041-9296-320F3D336965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7122E6A4-714B-8646-9C0B-9BB8D5016CC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27820" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27820" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Solicitudes Vales Grandeza" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Solicitudes Vales Grandeza'!$A$2:$AC$48</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Solicitudes Vales Grandeza'!$A$2:$AE$48</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Solicitudes Vales Grandeza'!$2:$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>NO.</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Celular</t>
   </si>
   <si>
-    <t>Correo</t>
-  </si>
-  <si>
     <t>CP</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>Incidencia</t>
   </si>
   <si>
-    <t>ListaParaEnviar</t>
-  </si>
-  <si>
     <t>Enlace</t>
   </si>
   <si>
@@ -121,6 +115,18 @@
   </si>
   <si>
     <t>FolioSolicitud</t>
+  </si>
+  <si>
+    <t>Remesa</t>
+  </si>
+  <si>
+    <t>Serie Inicial</t>
+  </si>
+  <si>
+    <t>Serie Final</t>
+  </si>
+  <si>
+    <t>Devuelto</t>
   </si>
 </sst>
 </file>
@@ -591,10 +597,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC10"/>
+  <dimension ref="A1:AE10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -617,14 +623,16 @@
     <col min="17" max="17" width="25.83203125" customWidth="1"/>
     <col min="18" max="20" width="30.83203125" customWidth="1"/>
     <col min="21" max="22" width="12.83203125" customWidth="1"/>
-    <col min="23" max="23" width="33.33203125" customWidth="1"/>
-    <col min="24" max="24" width="29.5" customWidth="1"/>
-    <col min="25" max="26" width="14.5" customWidth="1"/>
-    <col min="27" max="28" width="15.83203125" customWidth="1"/>
-    <col min="29" max="29" width="18.6640625" customWidth="1"/>
+    <col min="23" max="23" width="14.33203125" customWidth="1"/>
+    <col min="24" max="24" width="19.33203125" customWidth="1"/>
+    <col min="25" max="25" width="10.83203125" customWidth="1"/>
+    <col min="26" max="26" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.83203125" customWidth="1"/>
+    <col min="29" max="31" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -654,8 +662,10 @@
       <c r="AA1" s="3"/>
       <c r="AB1" s="3"/>
       <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -685,8 +695,10 @@
       <c r="AA2" s="4"/>
       <c r="AB2" s="4"/>
       <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -716,8 +728,10 @@
       <c r="AA3" s="3"/>
       <c r="AB3" s="3"/>
       <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -747,8 +761,10 @@
       <c r="AA4" s="3"/>
       <c r="AB4" s="3"/>
       <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -778,8 +794,10 @@
       <c r="AA5" s="3"/>
       <c r="AB5" s="3"/>
       <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -809,8 +827,10 @@
       <c r="AA6" s="12"/>
       <c r="AB6" s="12"/>
       <c r="AC6" s="12"/>
+      <c r="AD6" s="12"/>
+      <c r="AE6" s="12"/>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -840,8 +860,10 @@
       <c r="AA7" s="3"/>
       <c r="AB7" s="3"/>
       <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -871,8 +893,10 @@
       <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
       <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -902,97 +926,105 @@
       <c r="AA9" s="3"/>
       <c r="AB9" s="3"/>
       <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
     </row>
-    <row r="10" spans="1:29" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" s="11" t="s">
+      <c r="J10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="K10" s="11" t="s">
+      <c r="L10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="O10" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="P10" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="R10" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="S10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="T10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="U10" s="11" t="s">
         <v>10</v>
-      </c>
-      <c r="L10" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M10" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="N10" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="O10" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="P10" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q10" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="R10" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="S10" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="T10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="U10" s="11" t="s">
-        <v>11</v>
       </c>
       <c r="V10" s="11" t="s">
         <v>1</v>
       </c>
       <c r="W10" s="11" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="X10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC10" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD10" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE10" s="11" t="s">
         <v>14</v>
-      </c>
-      <c r="Y10" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z10" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA10" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB10" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC10" s="11" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="W6:AC6"/>
+    <mergeCell ref="W6:AE6"/>
   </mergeCells>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
   <pageSetup scale="30" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>